<commit_message>
Corrected Feb-Mar 2024 data
</commit_message>
<xml_diff>
--- a/data/monthly_es_rules/monthly_econ_significant_rules_by_presidential_month.xlsx
+++ b/data/monthly_es_rules/monthly_econ_significant_rules_by_presidential_month.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\GWRSC\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezd\Documents\GitHub\Reg-Stats\data\monthly_es_rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1032D0-B42A-418E-9196-0D76316265F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC45160-A08C-460F-974A-F99F75627E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly_econ_significant_rul" sheetId="1" r:id="rId1"/>
@@ -1591,10 +1591,10 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>34</c:v>
@@ -2917,7 +2917,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{769F7AA1-03EB-4CEF-BD18-3786E81FF1B8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3107,7 +3107,7 @@
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Updated: May 3, 2024</a:t>
+            <a:t>Updated: May 8, 2024</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
@@ -3438,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4588,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S39" s="1"/>
     </row>
@@ -4618,7 +4618,7 @@
         <v>5</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S40" s="1"/>
     </row>
@@ -5912,7 +5912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B7D354-9164-4D5E-9812-4C9860F64625}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -5943,6 +5945,7 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <f>monthly_econ_significant_rul!I3</f>
         <v>6</v>
       </c>
     </row>
@@ -5954,6 +5957,7 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <f>monthly_econ_significant_rul!I4</f>
         <v>4</v>
       </c>
     </row>
@@ -5965,6 +5969,7 @@
         <v>3</v>
       </c>
       <c r="C5">
+        <f>monthly_econ_significant_rul!I5</f>
         <v>2</v>
       </c>
     </row>
@@ -5976,6 +5981,7 @@
         <v>4</v>
       </c>
       <c r="C6">
+        <f>monthly_econ_significant_rul!I6</f>
         <v>10</v>
       </c>
     </row>
@@ -5987,6 +5993,7 @@
         <v>5</v>
       </c>
       <c r="C7">
+        <f>monthly_econ_significant_rul!I7</f>
         <v>2</v>
       </c>
     </row>
@@ -5998,6 +6005,7 @@
         <v>6</v>
       </c>
       <c r="C8">
+        <f>monthly_econ_significant_rul!I8</f>
         <v>8</v>
       </c>
     </row>
@@ -6009,6 +6017,7 @@
         <v>7</v>
       </c>
       <c r="C9">
+        <f>monthly_econ_significant_rul!I9</f>
         <v>10</v>
       </c>
     </row>
@@ -6020,6 +6029,7 @@
         <v>8</v>
       </c>
       <c r="C10">
+        <f>monthly_econ_significant_rul!I10</f>
         <v>3</v>
       </c>
     </row>
@@ -6031,6 +6041,7 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <f>monthly_econ_significant_rul!I11</f>
         <v>6</v>
       </c>
     </row>
@@ -6042,6 +6053,7 @@
         <v>10</v>
       </c>
       <c r="C12">
+        <f>monthly_econ_significant_rul!I12</f>
         <v>10</v>
       </c>
     </row>
@@ -6053,6 +6065,7 @@
         <v>11</v>
       </c>
       <c r="C13">
+        <f>monthly_econ_significant_rul!I13</f>
         <v>5</v>
       </c>
     </row>
@@ -6064,6 +6077,7 @@
         <v>12</v>
       </c>
       <c r="C14">
+        <f>monthly_econ_significant_rul!I14</f>
         <v>3</v>
       </c>
     </row>
@@ -6075,6 +6089,7 @@
         <v>13</v>
       </c>
       <c r="C15">
+        <f>monthly_econ_significant_rul!I15</f>
         <v>2</v>
       </c>
     </row>
@@ -6086,6 +6101,7 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <f>monthly_econ_significant_rul!I16</f>
         <v>2</v>
       </c>
     </row>
@@ -6097,6 +6113,7 @@
         <v>15</v>
       </c>
       <c r="C17">
+        <f>monthly_econ_significant_rul!I17</f>
         <v>3</v>
       </c>
     </row>
@@ -6108,6 +6125,7 @@
         <v>16</v>
       </c>
       <c r="C18">
+        <f>monthly_econ_significant_rul!I18</f>
         <v>8</v>
       </c>
     </row>
@@ -6119,6 +6137,7 @@
         <v>17</v>
       </c>
       <c r="C19">
+        <f>monthly_econ_significant_rul!I19</f>
         <v>0</v>
       </c>
     </row>
@@ -6130,6 +6149,7 @@
         <v>18</v>
       </c>
       <c r="C20">
+        <f>monthly_econ_significant_rul!I20</f>
         <v>4</v>
       </c>
     </row>
@@ -6141,6 +6161,7 @@
         <v>19</v>
       </c>
       <c r="C21">
+        <f>monthly_econ_significant_rul!I21</f>
         <v>5</v>
       </c>
     </row>
@@ -6152,6 +6173,7 @@
         <v>20</v>
       </c>
       <c r="C22">
+        <f>monthly_econ_significant_rul!I22</f>
         <v>4</v>
       </c>
     </row>
@@ -6163,6 +6185,7 @@
         <v>21</v>
       </c>
       <c r="C23">
+        <f>monthly_econ_significant_rul!I23</f>
         <v>6</v>
       </c>
     </row>
@@ -6174,6 +6197,7 @@
         <v>22</v>
       </c>
       <c r="C24">
+        <f>monthly_econ_significant_rul!I24</f>
         <v>7</v>
       </c>
     </row>
@@ -6185,6 +6209,7 @@
         <v>23</v>
       </c>
       <c r="C25">
+        <f>monthly_econ_significant_rul!I25</f>
         <v>4</v>
       </c>
     </row>
@@ -6196,6 +6221,7 @@
         <v>24</v>
       </c>
       <c r="C26">
+        <f>monthly_econ_significant_rul!I26</f>
         <v>4</v>
       </c>
     </row>
@@ -6207,6 +6233,7 @@
         <v>25</v>
       </c>
       <c r="C27">
+        <f>monthly_econ_significant_rul!I27</f>
         <v>2</v>
       </c>
     </row>
@@ -6218,6 +6245,7 @@
         <v>26</v>
       </c>
       <c r="C28">
+        <f>monthly_econ_significant_rul!I28</f>
         <v>1</v>
       </c>
     </row>
@@ -6229,6 +6257,7 @@
         <v>27</v>
       </c>
       <c r="C29">
+        <f>monthly_econ_significant_rul!I29</f>
         <v>3</v>
       </c>
     </row>
@@ -6240,6 +6269,7 @@
         <v>28</v>
       </c>
       <c r="C30">
+        <f>monthly_econ_significant_rul!I30</f>
         <v>3</v>
       </c>
     </row>
@@ -6251,6 +6281,7 @@
         <v>29</v>
       </c>
       <c r="C31">
+        <f>monthly_econ_significant_rul!I31</f>
         <v>4</v>
       </c>
     </row>
@@ -6262,6 +6293,7 @@
         <v>30</v>
       </c>
       <c r="C32">
+        <f>monthly_econ_significant_rul!I32</f>
         <v>5</v>
       </c>
     </row>
@@ -6273,6 +6305,7 @@
         <v>31</v>
       </c>
       <c r="C33">
+        <f>monthly_econ_significant_rul!I33</f>
         <v>12</v>
       </c>
     </row>
@@ -6284,6 +6317,7 @@
         <v>32</v>
       </c>
       <c r="C34">
+        <f>monthly_econ_significant_rul!I34</f>
         <v>12</v>
       </c>
     </row>
@@ -6295,6 +6329,7 @@
         <v>33</v>
       </c>
       <c r="C35">
+        <f>monthly_econ_significant_rul!I35</f>
         <v>9</v>
       </c>
     </row>
@@ -6306,6 +6341,7 @@
         <v>34</v>
       </c>
       <c r="C36">
+        <f>monthly_econ_significant_rul!I36</f>
         <v>10</v>
       </c>
     </row>
@@ -6317,6 +6353,7 @@
         <v>35</v>
       </c>
       <c r="C37">
+        <f>monthly_econ_significant_rul!I37</f>
         <v>8</v>
       </c>
     </row>
@@ -6328,6 +6365,7 @@
         <v>36</v>
       </c>
       <c r="C38">
+        <f>monthly_econ_significant_rul!I38</f>
         <v>9</v>
       </c>
     </row>
@@ -6339,7 +6377,8 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>7</v>
+        <f>monthly_econ_significant_rul!I39</f>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -6350,7 +6389,8 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <f>monthly_econ_significant_rul!I40</f>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -6361,6 +6401,7 @@
         <v>39</v>
       </c>
       <c r="C41">
+        <f>monthly_econ_significant_rul!I41</f>
         <v>34</v>
       </c>
     </row>
@@ -6446,7 +6487,7 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6478,6 +6519,7 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <f>monthly_econ_significant_rul!G3</f>
         <v>2</v>
       </c>
     </row>
@@ -6489,6 +6531,7 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <f>monthly_econ_significant_rul!G4</f>
         <v>4</v>
       </c>
     </row>
@@ -6500,6 +6543,7 @@
         <v>3</v>
       </c>
       <c r="C5">
+        <f>monthly_econ_significant_rul!G5</f>
         <v>3</v>
       </c>
     </row>
@@ -6511,6 +6555,7 @@
         <v>4</v>
       </c>
       <c r="C6">
+        <f>monthly_econ_significant_rul!G6</f>
         <v>2</v>
       </c>
     </row>
@@ -6522,6 +6567,7 @@
         <v>5</v>
       </c>
       <c r="C7">
+        <f>monthly_econ_significant_rul!G7</f>
         <v>2</v>
       </c>
     </row>
@@ -6533,6 +6579,7 @@
         <v>6</v>
       </c>
       <c r="C8">
+        <f>monthly_econ_significant_rul!G8</f>
         <v>7</v>
       </c>
     </row>
@@ -6544,6 +6591,7 @@
         <v>7</v>
       </c>
       <c r="C9">
+        <f>monthly_econ_significant_rul!G9</f>
         <v>5</v>
       </c>
     </row>
@@ -6555,6 +6603,7 @@
         <v>8</v>
       </c>
       <c r="C10">
+        <f>monthly_econ_significant_rul!G10</f>
         <v>2</v>
       </c>
     </row>
@@ -6566,6 +6615,7 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <f>monthly_econ_significant_rul!G11</f>
         <v>4</v>
       </c>
     </row>
@@ -6577,6 +6627,7 @@
         <v>10</v>
       </c>
       <c r="C12">
+        <f>monthly_econ_significant_rul!G12</f>
         <v>9</v>
       </c>
     </row>
@@ -6588,6 +6639,7 @@
         <v>11</v>
       </c>
       <c r="C13">
+        <f>monthly_econ_significant_rul!G13</f>
         <v>6</v>
       </c>
     </row>
@@ -6599,6 +6651,7 @@
         <v>12</v>
       </c>
       <c r="C14">
+        <f>monthly_econ_significant_rul!G14</f>
         <v>6</v>
       </c>
     </row>
@@ -6610,6 +6663,7 @@
         <v>13</v>
       </c>
       <c r="C15">
+        <f>monthly_econ_significant_rul!G15</f>
         <v>2</v>
       </c>
     </row>
@@ -6621,6 +6675,7 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <f>monthly_econ_significant_rul!G16</f>
         <v>7</v>
       </c>
     </row>
@@ -6632,6 +6687,7 @@
         <v>15</v>
       </c>
       <c r="C17">
+        <f>monthly_econ_significant_rul!G17</f>
         <v>8</v>
       </c>
     </row>
@@ -6643,6 +6699,7 @@
         <v>16</v>
       </c>
       <c r="C18">
+        <f>monthly_econ_significant_rul!G18</f>
         <v>8</v>
       </c>
     </row>
@@ -6654,6 +6711,7 @@
         <v>17</v>
       </c>
       <c r="C19">
+        <f>monthly_econ_significant_rul!G19</f>
         <v>7</v>
       </c>
     </row>
@@ -6665,6 +6723,7 @@
         <v>18</v>
       </c>
       <c r="C20">
+        <f>monthly_econ_significant_rul!G20</f>
         <v>8</v>
       </c>
     </row>
@@ -6676,6 +6735,7 @@
         <v>19</v>
       </c>
       <c r="C21">
+        <f>monthly_econ_significant_rul!G21</f>
         <v>7</v>
       </c>
     </row>
@@ -6687,6 +6747,7 @@
         <v>20</v>
       </c>
       <c r="C22">
+        <f>monthly_econ_significant_rul!G22</f>
         <v>5</v>
       </c>
     </row>
@@ -6698,6 +6759,7 @@
         <v>21</v>
       </c>
       <c r="C23">
+        <f>monthly_econ_significant_rul!G23</f>
         <v>7</v>
       </c>
     </row>
@@ -6709,6 +6771,7 @@
         <v>22</v>
       </c>
       <c r="C24">
+        <f>monthly_econ_significant_rul!G24</f>
         <v>5</v>
       </c>
     </row>
@@ -6720,6 +6783,7 @@
         <v>23</v>
       </c>
       <c r="C25">
+        <f>monthly_econ_significant_rul!G25</f>
         <v>4</v>
       </c>
     </row>
@@ -6731,6 +6795,7 @@
         <v>24</v>
       </c>
       <c r="C26">
+        <f>monthly_econ_significant_rul!G26</f>
         <v>2</v>
       </c>
     </row>
@@ -6742,6 +6807,7 @@
         <v>25</v>
       </c>
       <c r="C27">
+        <f>monthly_econ_significant_rul!G27</f>
         <v>4</v>
       </c>
     </row>
@@ -6753,6 +6819,7 @@
         <v>26</v>
       </c>
       <c r="C28">
+        <f>monthly_econ_significant_rul!G28</f>
         <v>7</v>
       </c>
     </row>
@@ -6764,6 +6831,7 @@
         <v>27</v>
       </c>
       <c r="C29">
+        <f>monthly_econ_significant_rul!G29</f>
         <v>5</v>
       </c>
     </row>
@@ -6775,6 +6843,7 @@
         <v>28</v>
       </c>
       <c r="C30">
+        <f>monthly_econ_significant_rul!G30</f>
         <v>3</v>
       </c>
     </row>
@@ -6786,6 +6855,7 @@
         <v>29</v>
       </c>
       <c r="C31">
+        <f>monthly_econ_significant_rul!G31</f>
         <v>6</v>
       </c>
     </row>
@@ -6797,6 +6867,7 @@
         <v>30</v>
       </c>
       <c r="C32">
+        <f>monthly_econ_significant_rul!G32</f>
         <v>2</v>
       </c>
     </row>
@@ -6808,6 +6879,7 @@
         <v>31</v>
       </c>
       <c r="C33">
+        <f>monthly_econ_significant_rul!G33</f>
         <v>6</v>
       </c>
     </row>
@@ -6819,6 +6891,7 @@
         <v>32</v>
       </c>
       <c r="C34">
+        <f>monthly_econ_significant_rul!G34</f>
         <v>7</v>
       </c>
     </row>
@@ -6830,6 +6903,7 @@
         <v>33</v>
       </c>
       <c r="C35">
+        <f>monthly_econ_significant_rul!G35</f>
         <v>1</v>
       </c>
     </row>
@@ -6841,6 +6915,7 @@
         <v>34</v>
       </c>
       <c r="C36">
+        <f>monthly_econ_significant_rul!G36</f>
         <v>7</v>
       </c>
     </row>
@@ -6852,6 +6927,7 @@
         <v>35</v>
       </c>
       <c r="C37">
+        <f>monthly_econ_significant_rul!G37</f>
         <v>3</v>
       </c>
     </row>
@@ -6863,6 +6939,7 @@
         <v>36</v>
       </c>
       <c r="C38">
+        <f>monthly_econ_significant_rul!G38</f>
         <v>3</v>
       </c>
     </row>
@@ -6874,6 +6951,7 @@
         <v>37</v>
       </c>
       <c r="C39">
+        <f>monthly_econ_significant_rul!G39</f>
         <v>3</v>
       </c>
     </row>
@@ -6885,6 +6963,7 @@
         <v>38</v>
       </c>
       <c r="C40">
+        <f>monthly_econ_significant_rul!G40</f>
         <v>5</v>
       </c>
     </row>
@@ -6896,6 +6975,7 @@
         <v>39</v>
       </c>
       <c r="C41">
+        <f>monthly_econ_significant_rul!G41</f>
         <v>4</v>
       </c>
     </row>
@@ -6907,6 +6987,7 @@
         <v>40</v>
       </c>
       <c r="C42">
+        <f>monthly_econ_significant_rul!G42</f>
         <v>8</v>
       </c>
     </row>
@@ -6918,6 +6999,7 @@
         <v>41</v>
       </c>
       <c r="C43">
+        <f>monthly_econ_significant_rul!G43</f>
         <v>2</v>
       </c>
     </row>
@@ -6929,6 +7011,7 @@
         <v>42</v>
       </c>
       <c r="C44">
+        <f>monthly_econ_significant_rul!G44</f>
         <v>0</v>
       </c>
     </row>
@@ -6940,6 +7023,7 @@
         <v>43</v>
       </c>
       <c r="C45">
+        <f>monthly_econ_significant_rul!G45</f>
         <v>6</v>
       </c>
     </row>
@@ -6951,6 +7035,7 @@
         <v>44</v>
       </c>
       <c r="C46">
+        <f>monthly_econ_significant_rul!G46</f>
         <v>6</v>
       </c>
     </row>
@@ -6962,6 +7047,7 @@
         <v>45</v>
       </c>
       <c r="C47">
+        <f>monthly_econ_significant_rul!G47</f>
         <v>2</v>
       </c>
     </row>
@@ -6973,6 +7059,7 @@
         <v>46</v>
       </c>
       <c r="C48">
+        <f>monthly_econ_significant_rul!G48</f>
         <v>5</v>
       </c>
     </row>
@@ -6984,6 +7071,7 @@
         <v>47</v>
       </c>
       <c r="C49">
+        <f>monthly_econ_significant_rul!G49</f>
         <v>1</v>
       </c>
     </row>
@@ -6995,6 +7083,7 @@
         <v>48</v>
       </c>
       <c r="C50">
+        <f>monthly_econ_significant_rul!G50</f>
         <v>7</v>
       </c>
     </row>
@@ -7006,6 +7095,7 @@
         <v>49</v>
       </c>
       <c r="C51">
+        <f>monthly_econ_significant_rul!G51</f>
         <v>5</v>
       </c>
     </row>
@@ -7017,6 +7107,7 @@
         <v>50</v>
       </c>
       <c r="C52">
+        <f>monthly_econ_significant_rul!G52</f>
         <v>4</v>
       </c>
     </row>
@@ -7028,6 +7119,7 @@
         <v>51</v>
       </c>
       <c r="C53">
+        <f>monthly_econ_significant_rul!G53</f>
         <v>3</v>
       </c>
     </row>
@@ -7039,6 +7131,7 @@
         <v>52</v>
       </c>
       <c r="C54">
+        <f>monthly_econ_significant_rul!G54</f>
         <v>4</v>
       </c>
     </row>
@@ -7050,6 +7143,7 @@
         <v>53</v>
       </c>
       <c r="C55">
+        <f>monthly_econ_significant_rul!G55</f>
         <v>2</v>
       </c>
     </row>
@@ -7061,6 +7155,7 @@
         <v>54</v>
       </c>
       <c r="C56">
+        <f>monthly_econ_significant_rul!G56</f>
         <v>6</v>
       </c>
     </row>
@@ -7072,6 +7167,7 @@
         <v>55</v>
       </c>
       <c r="C57">
+        <f>monthly_econ_significant_rul!G57</f>
         <v>8</v>
       </c>
     </row>
@@ -7083,6 +7179,7 @@
         <v>56</v>
       </c>
       <c r="C58">
+        <f>monthly_econ_significant_rul!G58</f>
         <v>5</v>
       </c>
     </row>
@@ -7094,6 +7191,7 @@
         <v>57</v>
       </c>
       <c r="C59">
+        <f>monthly_econ_significant_rul!G59</f>
         <v>2</v>
       </c>
     </row>
@@ -7105,6 +7203,7 @@
         <v>58</v>
       </c>
       <c r="C60">
+        <f>monthly_econ_significant_rul!G60</f>
         <v>3</v>
       </c>
     </row>
@@ -7116,6 +7215,7 @@
         <v>59</v>
       </c>
       <c r="C61">
+        <f>monthly_econ_significant_rul!G61</f>
         <v>8</v>
       </c>
     </row>
@@ -7127,6 +7227,7 @@
         <v>60</v>
       </c>
       <c r="C62">
+        <f>monthly_econ_significant_rul!G62</f>
         <v>4</v>
       </c>
     </row>
@@ -7138,6 +7239,7 @@
         <v>61</v>
       </c>
       <c r="C63">
+        <f>monthly_econ_significant_rul!G63</f>
         <v>2</v>
       </c>
     </row>
@@ -7149,6 +7251,7 @@
         <v>62</v>
       </c>
       <c r="C64">
+        <f>monthly_econ_significant_rul!G64</f>
         <v>5</v>
       </c>
     </row>
@@ -7160,6 +7263,7 @@
         <v>63</v>
       </c>
       <c r="C65">
+        <f>monthly_econ_significant_rul!G65</f>
         <v>5</v>
       </c>
     </row>
@@ -7171,6 +7275,7 @@
         <v>64</v>
       </c>
       <c r="C66">
+        <f>monthly_econ_significant_rul!G66</f>
         <v>7</v>
       </c>
     </row>
@@ -7182,6 +7287,7 @@
         <v>65</v>
       </c>
       <c r="C67">
+        <f>monthly_econ_significant_rul!G67</f>
         <v>2</v>
       </c>
     </row>
@@ -7193,6 +7299,7 @@
         <v>66</v>
       </c>
       <c r="C68">
+        <f>monthly_econ_significant_rul!G68</f>
         <v>2</v>
       </c>
     </row>
@@ -7204,6 +7311,7 @@
         <v>67</v>
       </c>
       <c r="C69">
+        <f>monthly_econ_significant_rul!G69</f>
         <v>10</v>
       </c>
     </row>
@@ -7215,6 +7323,7 @@
         <v>68</v>
       </c>
       <c r="C70">
+        <f>monthly_econ_significant_rul!G70</f>
         <v>4</v>
       </c>
     </row>
@@ -7226,6 +7335,7 @@
         <v>69</v>
       </c>
       <c r="C71">
+        <f>monthly_econ_significant_rul!G71</f>
         <v>4</v>
       </c>
     </row>
@@ -7237,6 +7347,7 @@
         <v>70</v>
       </c>
       <c r="C72">
+        <f>monthly_econ_significant_rul!G72</f>
         <v>5</v>
       </c>
     </row>
@@ -7248,6 +7359,7 @@
         <v>71</v>
       </c>
       <c r="C73">
+        <f>monthly_econ_significant_rul!G73</f>
         <v>7</v>
       </c>
     </row>
@@ -7259,6 +7371,7 @@
         <v>72</v>
       </c>
       <c r="C74">
+        <f>monthly_econ_significant_rul!G74</f>
         <v>4</v>
       </c>
     </row>
@@ -7270,6 +7383,7 @@
         <v>73</v>
       </c>
       <c r="C75">
+        <f>monthly_econ_significant_rul!G75</f>
         <v>3</v>
       </c>
     </row>
@@ -7281,6 +7395,7 @@
         <v>74</v>
       </c>
       <c r="C76">
+        <f>monthly_econ_significant_rul!G76</f>
         <v>1</v>
       </c>
     </row>
@@ -7292,6 +7407,7 @@
         <v>75</v>
       </c>
       <c r="C77">
+        <f>monthly_econ_significant_rul!G77</f>
         <v>3</v>
       </c>
     </row>
@@ -7303,6 +7419,7 @@
         <v>76</v>
       </c>
       <c r="C78">
+        <f>monthly_econ_significant_rul!G78</f>
         <v>3</v>
       </c>
     </row>
@@ -7314,6 +7431,7 @@
         <v>77</v>
       </c>
       <c r="C79">
+        <f>monthly_econ_significant_rul!G79</f>
         <v>7</v>
       </c>
     </row>
@@ -7325,6 +7443,7 @@
         <v>78</v>
       </c>
       <c r="C80">
+        <f>monthly_econ_significant_rul!G80</f>
         <v>5</v>
       </c>
     </row>
@@ -7336,6 +7455,7 @@
         <v>79</v>
       </c>
       <c r="C81">
+        <f>monthly_econ_significant_rul!G81</f>
         <v>5</v>
       </c>
     </row>
@@ -7347,6 +7467,7 @@
         <v>80</v>
       </c>
       <c r="C82">
+        <f>monthly_econ_significant_rul!G82</f>
         <v>5</v>
       </c>
     </row>
@@ -7358,6 +7479,7 @@
         <v>81</v>
       </c>
       <c r="C83">
+        <f>monthly_econ_significant_rul!G83</f>
         <v>10</v>
       </c>
     </row>
@@ -7369,6 +7491,7 @@
         <v>82</v>
       </c>
       <c r="C84">
+        <f>monthly_econ_significant_rul!G84</f>
         <v>8</v>
       </c>
     </row>
@@ -7380,6 +7503,7 @@
         <v>83</v>
       </c>
       <c r="C85">
+        <f>monthly_econ_significant_rul!G85</f>
         <v>9</v>
       </c>
     </row>
@@ -7391,6 +7515,7 @@
         <v>84</v>
       </c>
       <c r="C86">
+        <f>monthly_econ_significant_rul!G86</f>
         <v>3</v>
       </c>
     </row>
@@ -7402,6 +7527,7 @@
         <v>85</v>
       </c>
       <c r="C87">
+        <f>monthly_econ_significant_rul!G87</f>
         <v>4</v>
       </c>
     </row>
@@ -7413,6 +7539,7 @@
         <v>86</v>
       </c>
       <c r="C88">
+        <f>monthly_econ_significant_rul!G88</f>
         <v>8</v>
       </c>
     </row>
@@ -7424,6 +7551,7 @@
         <v>87</v>
       </c>
       <c r="C89">
+        <f>monthly_econ_significant_rul!G89</f>
         <v>3</v>
       </c>
     </row>
@@ -7435,6 +7563,7 @@
         <v>88</v>
       </c>
       <c r="C90">
+        <f>monthly_econ_significant_rul!G90</f>
         <v>8</v>
       </c>
     </row>
@@ -7446,6 +7575,7 @@
         <v>89</v>
       </c>
       <c r="C91">
+        <f>monthly_econ_significant_rul!G91</f>
         <v>8</v>
       </c>
     </row>
@@ -7457,6 +7587,7 @@
         <v>90</v>
       </c>
       <c r="C92">
+        <f>monthly_econ_significant_rul!G92</f>
         <v>5</v>
       </c>
     </row>
@@ -7468,6 +7599,7 @@
         <v>91</v>
       </c>
       <c r="C93">
+        <f>monthly_econ_significant_rul!G93</f>
         <v>10</v>
       </c>
     </row>
@@ -7479,6 +7611,7 @@
         <v>92</v>
       </c>
       <c r="C94">
+        <f>monthly_econ_significant_rul!G94</f>
         <v>4</v>
       </c>
     </row>
@@ -7490,6 +7623,7 @@
         <v>93</v>
       </c>
       <c r="C95">
+        <f>monthly_econ_significant_rul!G95</f>
         <v>9</v>
       </c>
     </row>
@@ -7501,6 +7635,7 @@
         <v>94</v>
       </c>
       <c r="C96">
+        <f>monthly_econ_significant_rul!G96</f>
         <v>11</v>
       </c>
     </row>
@@ -7512,6 +7647,7 @@
         <v>95</v>
       </c>
       <c r="C97">
+        <f>monthly_econ_significant_rul!G97</f>
         <v>14</v>
       </c>
     </row>
@@ -7523,6 +7659,7 @@
         <v>96</v>
       </c>
       <c r="C98">
+        <f>monthly_econ_significant_rul!G98</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>